<commit_message>
Commit with latest changes
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SodexoLatest\sample\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL-COMPUTER\git\sodexoMobileAutomationLatest\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="launch" sheetId="1" r:id="rId1"/>
-    <sheet name="createanaccount" sheetId="2" r:id="rId2"/>
+    <sheet name="login" sheetId="4" r:id="rId2"/>
+    <sheet name="createanaccount" sheetId="2" r:id="rId3"/>
+    <sheet name="menuData" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>email</t>
   </si>
@@ -42,9 +44,6 @@
     <t>location</t>
   </si>
   <si>
-    <t>Rio</t>
-  </si>
-  <si>
     <t>bitetest@gmail.com</t>
   </si>
   <si>
@@ -94,6 +93,24 @@
   </si>
   <si>
     <t>+1 301-987-4772</t>
+  </si>
+  <si>
+    <t>itemName</t>
+  </si>
+  <si>
+    <t>menuType</t>
+  </si>
+  <si>
+    <t>HBO Café</t>
+  </si>
+  <si>
+    <t>Bacon Slices</t>
+  </si>
+  <si>
+    <t>CHILDRENS</t>
+  </si>
+  <si>
+    <t>bitetest34@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -433,10 +450,13 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -445,7 +465,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -455,9 +475,46 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -475,10 +532,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -490,54 +547,54 @@
         <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
         <v>17</v>
       </c>
-      <c r="J1" t="s">
-        <v>18</v>
-      </c>
       <c r="K1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="J2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -547,4 +604,39 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Commit code with latest changes
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -5,17 +5,21 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL-COMPUTER\git\sodexoMobileAutomationLatest\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL-COMPUTER\git\Latest11may2020\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="launch" sheetId="1" r:id="rId1"/>
     <sheet name="login" sheetId="4" r:id="rId2"/>
     <sheet name="createanaccount" sheetId="2" r:id="rId3"/>
     <sheet name="menuData" sheetId="3" r:id="rId4"/>
+    <sheet name="orderdata" sheetId="5" r:id="rId5"/>
+    <sheet name="instructions" sheetId="6" r:id="rId6"/>
+    <sheet name="cardDetails" sheetId="7" r:id="rId7"/>
+    <sheet name="review" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>email</t>
   </si>
@@ -111,6 +115,48 @@
   </si>
   <si>
     <t>bitetest34@gmail.com</t>
+  </si>
+  <si>
+    <t>HBO Cafe Grill</t>
+  </si>
+  <si>
+    <t>Bacon</t>
+  </si>
+  <si>
+    <t>instructions</t>
+  </si>
+  <si>
+    <t>Placing order for 2 items from non veg</t>
+  </si>
+  <si>
+    <t>5399999999999999</t>
+  </si>
+  <si>
+    <t>cardnumber</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>cvv</t>
+  </si>
+  <si>
+    <t>zipcode</t>
+  </si>
+  <si>
+    <t>98760</t>
+  </si>
+  <si>
+    <t>Good menu</t>
+  </si>
+  <si>
+    <t>reviewcomments</t>
+  </si>
+  <si>
+    <t>menuorder</t>
+  </si>
+  <si>
+    <t>HBO</t>
   </si>
 </sst>
 </file>
@@ -610,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,4 +685,154 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2">
+        <v>11</v>
+      </c>
+      <c r="C2">
+        <v>2013</v>
+      </c>
+      <c r="D2">
+        <v>999</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
commit with ios code
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" tabRatio="932" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="launch" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,8 @@
     <sheet name="instructions" sheetId="6" r:id="rId6"/>
     <sheet name="cardDetails" sheetId="7" r:id="rId7"/>
     <sheet name="review" sheetId="8" r:id="rId8"/>
+    <sheet name="orderdata_ios" sheetId="9" r:id="rId9"/>
+    <sheet name="endtoend" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="63">
   <si>
     <t>email</t>
   </si>
@@ -157,6 +159,69 @@
   </si>
   <si>
     <t>HBO</t>
+  </si>
+  <si>
+    <t>Naan Bread</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> email</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> createAnAccountlbl</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nextletscreateaccountlbl</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> firstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">			lastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> password</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> verifyPwd</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> month</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">			phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> menuType</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> itemName</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> reviewcomments</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cardNum</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> YYYY</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cvv</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> zipcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testing review </t>
+  </si>
+  <si>
+    <t>CHILDRENS HOSPITAL</t>
   </si>
 </sst>
 </file>
@@ -519,12 +584,175 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:P1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>57</v>
+      </c>
+      <c r="R1" t="s">
+        <v>58</v>
+      </c>
+      <c r="S1" t="s">
+        <v>59</v>
+      </c>
+      <c r="T1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" t="s">
+        <v>61</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2">
+        <v>11</v>
+      </c>
+      <c r="R2">
+        <v>2013</v>
+      </c>
+      <c r="S2">
+        <v>999</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,7 +789,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,7 +885,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="B2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,7 +983,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,7 +1034,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -835,4 +1063,39 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>